<commit_message>
RTM for Build 10
</commit_message>
<xml_diff>
--- a/Test/Build 10/TASCore_Defect_Log_v2.0.xlsx
+++ b/Test/Build 10/TASCore_Defect_Log_v2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VHAISPFOWLDD\repos\mccf_tascore_documents\Test\TAS_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243A6481-7D5A-4ABB-BB71-95673A9E0620}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C42DAB-C1C2-4912-A2EF-67BD0D0DE58B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t>Department of Veterans Affairs</t>
   </si>
@@ -151,12 +151,6 @@
   </si>
   <si>
     <t xml:space="preserve">Updated new version #s post SwA </t>
-  </si>
-  <si>
-    <t>Version 4.0</t>
-  </si>
-  <si>
-    <t>May 17, 2019</t>
   </si>
   <si>
     <r>
@@ -253,8 +247,23 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> VAVLGateway_02.00.3_20190516_084015</t>
+      <t xml:space="preserve"> VAVLGateway_02.00.3_20190516_085649</t>
     </r>
+  </si>
+  <si>
+    <t>May 20, 2019</t>
+  </si>
+  <si>
+    <t>Version 5.0</t>
+  </si>
+  <si>
+    <t>05-20-2019</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated VistALink version number </t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82CCFCA9-7609-4BE4-98C5-F41705754B55}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -1178,7 +1189,7 @@
     </row>
     <row r="3" spans="1:7" s="9" customFormat="1" ht="70.25" customHeight="1">
       <c r="A3" s="27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="9" customFormat="1" ht="17.5" customHeight="1">
@@ -1221,7 +1232,7 @@
     </row>
     <row r="16" spans="1:7" s="9" customFormat="1" ht="17" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:1" s="9" customFormat="1" ht="15" customHeight="1" thickBot="1">
@@ -1235,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
@@ -1275,13 +1286,13 @@
     </row>
     <row r="3" spans="1:4" s="32" customFormat="1" ht="15.75" customHeight="1">
       <c r="A3" s="29" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D3" s="31" t="s">
         <v>17</v>
@@ -1289,54 +1300,68 @@
     </row>
     <row r="4" spans="1:4" s="32" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="29" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D4" s="31" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A5" s="14">
+    <row r="5" spans="1:4" s="32" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A5" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A6" s="14">
         <v>43593</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B6" s="15">
         <v>2</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D6" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="18">
+    <row r="7" spans="1:4" s="10" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A7" s="18">
         <v>43581</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B7" s="19">
         <v>1</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>